<commit_message>
EPBDS-8861 Reference to cell doesn't work properly in Test table, if type of input value is Custom SpreadsheetResult
</commit_message>
<xml_diff>
--- a/STUDIO/org.openl.rules.test/test-resources/functionality/EPBDS-7313_SR_SimplifiedRef.xlsx
+++ b/STUDIO/org.openl.rules.test/test-resources/functionality/EPBDS-7313_SR_SimplifiedRef.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21901"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46E5C39A-7622-4468-AE3F-AD326ECE8FC4}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E52963A0-7254-4476-8C00-B6FB0B99BB4C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4920" yWindow="1950" windowWidth="23880" windowHeight="16965" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="225" yWindow="90" windowWidth="31815" windowHeight="20565" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Test1" sheetId="11" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="35">
   <si>
     <t>Step</t>
   </si>
@@ -81,9 +81,6 @@
     <t>Result</t>
   </si>
   <si>
-    <t>_res_.$A.$B</t>
-  </si>
-  <si>
     <t>_context_.usState</t>
   </si>
   <si>
@@ -102,12 +99,6 @@
     <t>= Inner2()</t>
   </si>
   <si>
-    <t>_res_.$B</t>
-  </si>
-  <si>
-    <t>_res_.$C</t>
-  </si>
-  <si>
     <t>= $A.$C</t>
   </si>
   <si>
@@ -136,17 +127,25 @@
   </si>
   <si>
     <t>Test Main4 Main4Test</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> _res_.$A.$B</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> _res_.$B</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> _res_.$C</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
-      <color theme="1" rgb="000000"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -170,17 +169,17 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -521,14 +520,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAF3A826-B4DF-46A0-BED0-58E2DFF1F6CD}">
   <dimension ref="A3:H44"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="I29" sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D46" sqref="D46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" customWidth="true" width="30.28515625" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="41.42578125" collapsed="true"/>
+    <col min="3" max="3" width="30.28515625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="41.42578125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:8" x14ac:dyDescent="0.25">
@@ -883,16 +882,16 @@
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B37" s="1"/>
       <c r="C37" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>16</v>
+        <v>32</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B38" s="1"/>
       <c r="C38" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D38" s="1" t="s">
         <v>15</v>
@@ -946,20 +945,20 @@
   <dimension ref="C5:F40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="F37" sqref="F37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" style="1" width="9.140625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="1" width="30.28515625" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="1" width="41.42578125" collapsed="true"/>
-    <col min="5" max="16384" style="1" width="9.140625" collapsed="true"/>
+    <col min="1" max="2" width="9.140625" style="1" collapsed="1"/>
+    <col min="3" max="3" width="30.28515625" style="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="41.42578125" style="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="16384" width="9.140625" style="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="5" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C5" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="3:5" x14ac:dyDescent="0.25">
@@ -975,7 +974,7 @@
         <v>8</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="8" spans="3:5" x14ac:dyDescent="0.25">
@@ -991,15 +990,15 @@
         <v>10</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="15" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C15" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D15" s="4"/>
-      <c r="E15" s="4"/>
+      <c r="C15" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
     </row>
     <row r="16" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C16" s="1" t="s">
@@ -1050,11 +1049,11 @@
     </row>
     <row r="21" spans="3:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="24" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C24" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D24" s="4"/>
-      <c r="E24" s="4"/>
+      <c r="C24" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D24" s="5"/>
+      <c r="E24" s="5"/>
     </row>
     <row r="25" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C25" s="1" t="s">
@@ -1072,7 +1071,7 @@
         <v>0</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E26" s="2"/>
     </row>
@@ -1104,30 +1103,30 @@
       <c r="E29" s="2"/>
     </row>
     <row r="36" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C36" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="D36" s="4"/>
-      <c r="E36" s="4"/>
-      <c r="F36" s="4"/>
+      <c r="C36" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D36" s="5"/>
+      <c r="E36" s="5"/>
+      <c r="F36" s="5"/>
     </row>
     <row r="37" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C37" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>24</v>
+        <v>34</v>
       </c>
     </row>
     <row r="38" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C38" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D38" s="1" t="s">
         <v>9</v>
@@ -1182,20 +1181,20 @@
   <dimension ref="C5:F40"/>
   <sheetViews>
     <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24:F27"/>
+      <selection activeCell="D48" sqref="D48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" style="1" width="9.140625" collapsed="false"/>
-    <col min="3" max="3" customWidth="true" style="1" width="30.28515625" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="1" width="41.42578125" collapsed="true"/>
-    <col min="5" max="16384" style="1" width="9.140625" collapsed="false"/>
+    <col min="1" max="2" width="9.140625" style="1"/>
+    <col min="3" max="3" width="30.28515625" style="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="41.42578125" style="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="5" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C5" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6" spans="3:6" x14ac:dyDescent="0.25">
@@ -1217,7 +1216,7 @@
         <v>1</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E7" s="3" t="s">
         <v>11</v>
@@ -1231,7 +1230,7 @@
     </row>
     <row r="15" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C15" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="16" spans="3:6" x14ac:dyDescent="0.25">
@@ -1276,7 +1275,7 @@
     <row r="21" spans="3:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="24" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C24" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="25" spans="3:6" x14ac:dyDescent="0.25">
@@ -1320,20 +1319,20 @@
     </row>
     <row r="36" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C36" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="37" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C37" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>16</v>
+        <v>32</v>
       </c>
     </row>
     <row r="38" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C38" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D38" s="1" t="s">
         <v>15</v>
@@ -1364,21 +1363,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EECAD6CB-8D4B-44A8-92E4-3D558101CFD5}">
   <dimension ref="C5:F40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F37" sqref="F37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" style="1" width="9.140625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="1" width="30.28515625" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="1" width="41.42578125" collapsed="true"/>
-    <col min="5" max="16384" style="1" width="9.140625" collapsed="true"/>
+    <col min="1" max="2" width="9.140625" style="1" collapsed="1"/>
+    <col min="3" max="3" width="30.28515625" style="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="41.42578125" style="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="16384" width="9.140625" style="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="5" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C5" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="3:5" x14ac:dyDescent="0.25">
@@ -1394,7 +1393,7 @@
         <v>8</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="8" spans="3:5" x14ac:dyDescent="0.25">
@@ -1410,12 +1409,12 @@
         <v>10</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="15" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C15" s="2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
@@ -1444,7 +1443,7 @@
       <c r="C18" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D18" s="5" t="s">
+      <c r="D18" s="4" t="s">
         <v>12</v>
       </c>
       <c r="E18" s="2"/>
@@ -1470,7 +1469,7 @@
     <row r="21" spans="3:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="24" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C24" s="2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
@@ -1494,14 +1493,14 @@
         <v>1</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="27" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C27" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D27" s="5" t="s">
+      <c r="D27" s="4" t="s">
         <v>12</v>
       </c>
       <c r="E27" s="2"/>
@@ -1525,30 +1524,30 @@
       <c r="E29" s="2"/>
     </row>
     <row r="36" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C36" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="D36" s="4"/>
-      <c r="E36" s="4"/>
-      <c r="F36" s="4"/>
+      <c r="C36" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D36" s="5"/>
+      <c r="E36" s="5"/>
+      <c r="F36" s="5"/>
     </row>
     <row r="37" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C37" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>24</v>
+        <v>34</v>
       </c>
     </row>
     <row r="38" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C38" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D38" s="1" t="s">
         <v>9</v>
@@ -1578,9 +1577,6 @@
       <c r="C40" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D40" s="1"/>
-      <c r="E40" s="1"/>
-      <c r="F40" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>